<commit_message>
Anh Minh Còi :))
</commit_message>
<xml_diff>
--- a/Documents/RaSoatNghiepVu.xlsx
+++ b/Documents/RaSoatNghiepVu.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>NỘI DUNG RÀ SOÁT NGHIỆP VỤ BẢO LONG ĐƯỜNG KINH BẮC</t>
   </si>
@@ -156,6 +156,70 @@
   </si>
   <si>
     <t>- Chưa có thông tin người chỉ định</t>
+  </si>
+  <si>
+    <t>Hội viên</t>
+  </si>
+  <si>
+    <t>Thống kê chung</t>
+  </si>
+  <si>
+    <r>
+      <t>- Tên tài khoản
+- Họ và tên
+- Số điểm hiện tại
+- Cấp bậc
+- Tổng số người bên trái, bên phải
+- Khi đã đủ 7 người bên trái, 7 người bên phải xét xem đã nhận tiền chưa (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>Thông báo "Đã nhận tiền" hay "Chưa nhận tiền"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Palatino Linotype"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Cây khách hàng</t>
+  </si>
+  <si>
+    <t>- Thêm thông tin khách hàng
+    + Tài khoản
+    + Cấp bậc
+    + Số khách hàng cấp dưới</t>
+  </si>
+  <si>
+    <t>Quy đổi điêm</t>
+  </si>
+  <si>
+    <t>Quy đổi điểm</t>
+  </si>
+  <si>
+    <t>- Thêm tìm kiếm thông tin quy đổi theo thời gian quy đổi (thời gian bắt đầu, thời gian kết thúc)
+- Danh sách các lượt quy đổi theo thời gian (số điểm quy đổi, thời gian giao dịch, trạng thái)</t>
+  </si>
+  <si>
+    <t>Điểm thưởng</t>
+  </si>
+  <si>
+    <t>- Tìm kiếm theo thời gian thưởng
+- Thông tin điểm thưởng: số điểm thưởng, loại (trực tiếp, gián tiếp), thưởng từ ai, thời gian</t>
+  </si>
+  <si>
+    <t>Yêu cầu lên cấp</t>
   </si>
 </sst>
 </file>
@@ -211,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -234,96 +298,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,72 +317,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -705,28 +662,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" style="10" customWidth="1"/>
     <col min="10" max="10" width="0.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -734,284 +691,452 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-    </row>
-    <row r="5" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="15" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
+    <row r="6" spans="1:10" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="A6" s="19">
         <v>1</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.35">
-      <c r="A7" s="16">
+    <row r="7" spans="1:10" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+      <c r="A7" s="19">
         <v>2</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.35">
-      <c r="A8" s="16">
+    <row r="8" spans="1:10" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+      <c r="A8" s="19">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.35">
-      <c r="A9" s="16">
+    <row r="9" spans="1:10" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="A9" s="19">
         <v>4</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.35">
-      <c r="A10" s="16">
+    <row r="10" spans="1:10" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="A10" s="19">
         <v>5</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="16">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="19">
         <v>1</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="16">
+    <row r="13" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="19">
         <v>2</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="16">
+    <row r="14" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="19">
         <v>3</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="16">
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="19">
         <v>4</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="16">
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="19">
         <v>5</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
+    <row r="17" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="19">
         <v>6</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="16">
+    <row r="18" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="19">
         <v>7</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:4" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-    </row>
-    <row r="20" spans="1:4" s="7" customFormat="1" ht="54" x14ac:dyDescent="0.35">
-      <c r="A20" s="16">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="A20" s="19">
         <v>1</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.35">
-      <c r="A21" s="16">
+    <row r="21" spans="1:4" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="A21" s="19">
         <v>2</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="21">
+    <row r="22" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="19">
         <v>3</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+    <row r="23" spans="1:4" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A23" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="1:4" s="6" customFormat="1" ht="144" x14ac:dyDescent="0.35">
+      <c r="A24" s="19">
+        <v>1</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+      <c r="A25" s="19">
+        <v>2</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+      <c r="A26" s="19">
+        <v>3</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="6" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="A27" s="19">
+        <v>4</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="19">
+        <v>5</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="7"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="7"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="7"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="7"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="7"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="7"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="7"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A36" s="7"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="7"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="7"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="7"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="7"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="7"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="7"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="7"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A47" s="7"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A49" s="7"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>